<commit_message>
Updated to the final versions
</commit_message>
<xml_diff>
--- a/Unique_AE_Terms/Unique_AE-term-trimming_summary_report_1208.xlsx
+++ b/Unique_AE_Terms/Unique_AE-term-trimming_summary_report_1208.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -387,7 +387,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>OUTPUT3.xlsx</t>
+          <t>OUTPUT6.xlsx</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -396,19 +396,19 @@
         </is>
       </c>
       <c r="C2">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="D2">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E2">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>OUTPUT3.xlsx</t>
+          <t>OUTPUT6.xlsx</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -417,19 +417,19 @@
         </is>
       </c>
       <c r="C3">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="D3">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>60</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>OUTPUT3.xlsx</t>
+          <t>OUTPUT6.xlsx</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -438,19 +438,19 @@
         </is>
       </c>
       <c r="C4">
-        <v>134</v>
+        <v>101</v>
       </c>
       <c r="D4">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E4">
-        <v>97</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>OUTPUT4.xlsx</t>
+          <t>OUTPUT9.xlsx</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -459,19 +459,19 @@
         </is>
       </c>
       <c r="C5">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="D5">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E5">
-        <v>76</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>OUTPUT4.xlsx</t>
+          <t>OUTPUT9.xlsx</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -480,19 +480,19 @@
         </is>
       </c>
       <c r="C6">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="D6">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E6">
-        <v>45</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>OUTPUT4.xlsx</t>
+          <t>OUTPUT9.xlsx</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -501,453 +501,75 @@
         </is>
       </c>
       <c r="C7">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="D7">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E7">
-        <v>73</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>OUTPUT5.xlsx</t>
+          <t>OUTPUT9.xlsx</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>PFIZER-BIONTECH</t>
+          <t>NOVAVAX</t>
         </is>
       </c>
       <c r="C8">
-        <v>101</v>
+        <v>165</v>
       </c>
       <c r="D8">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="E8">
-        <v>66</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>OUTPUT5.xlsx</t>
+          <t>OUTPUT9.xlsx</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>MODERNA</t>
+          <t>MODERNA BIVALENT</t>
         </is>
       </c>
       <c r="C9">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="D9">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="E9">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>OUTPUT5.xlsx</t>
+          <t>OUTPUT9.xlsx</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>PFIZER-BIONTECH BIVALENT</t>
         </is>
       </c>
       <c r="C10">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="D10">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="E10">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>OUTPUT6.xlsx</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>PFIZER-BIONTECH</t>
-        </is>
-      </c>
-      <c r="C11">
-        <v>99</v>
-      </c>
-      <c r="D11">
-        <v>35</v>
-      </c>
-      <c r="E11">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>OUTPUT6.xlsx</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>MODERNA</t>
-        </is>
-      </c>
-      <c r="C12">
-        <v>33</v>
-      </c>
-      <c r="D12">
-        <v>10</v>
-      </c>
-      <c r="E12">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>OUTPUT6.xlsx</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>JANSSEN</t>
-        </is>
-      </c>
-      <c r="C13">
-        <v>101</v>
-      </c>
-      <c r="D13">
-        <v>41</v>
-      </c>
-      <c r="E13">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>OUTPUT7.xlsx</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>PFIZER-BIONTECH</t>
-        </is>
-      </c>
-      <c r="C14">
-        <v>83</v>
-      </c>
-      <c r="D14">
-        <v>35</v>
-      </c>
-      <c r="E14">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>OUTPUT7.xlsx</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>MODERNA</t>
-        </is>
-      </c>
-      <c r="C15">
-        <v>20</v>
-      </c>
-      <c r="D15">
-        <v>6</v>
-      </c>
-      <c r="E15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>OUTPUT7.xlsx</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>JANSSEN</t>
-        </is>
-      </c>
-      <c r="C16">
-        <v>91</v>
-      </c>
-      <c r="D16">
-        <v>36</v>
-      </c>
-      <c r="E16">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>OUTPUT8.xlsx</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>PFIZER-BIONTECH</t>
-        </is>
-      </c>
-      <c r="C17">
-        <v>25</v>
-      </c>
-      <c r="D17">
-        <v>17</v>
-      </c>
-      <c r="E17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>OUTPUT8.xlsx</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>MODERNA</t>
-        </is>
-      </c>
-      <c r="C18">
-        <v>11</v>
-      </c>
-      <c r="D18">
-        <v>7</v>
-      </c>
-      <c r="E18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>OUTPUT8.xlsx</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>JANSSEN</t>
-        </is>
-      </c>
-      <c r="C19">
-        <v>182</v>
-      </c>
-      <c r="D19">
-        <v>61</v>
-      </c>
-      <c r="E19">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>OUTPUT8.xlsx</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>NOVAVAX</t>
-        </is>
-      </c>
-      <c r="C20">
-        <v>127</v>
-      </c>
-      <c r="D20">
-        <v>29</v>
-      </c>
-      <c r="E20">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>OUTPUT8.xlsx</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>MODERNA BIVALENT</t>
-        </is>
-      </c>
-      <c r="C21">
-        <v>30</v>
-      </c>
-      <c r="D21">
-        <v>12</v>
-      </c>
-      <c r="E21">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>OUTPUT8.xlsx</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>PFIZER-BIONTECH BIVALENT</t>
-        </is>
-      </c>
-      <c r="C22">
-        <v>41</v>
-      </c>
-      <c r="D22">
-        <v>14</v>
-      </c>
-      <c r="E22">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>OUTPUT9.xlsx</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>PFIZER-BIONTECH</t>
-        </is>
-      </c>
-      <c r="C23">
-        <v>83</v>
-      </c>
-      <c r="D23">
-        <v>35</v>
-      </c>
-      <c r="E23">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>OUTPUT9.xlsx</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>MODERNA</t>
-        </is>
-      </c>
-      <c r="C24">
-        <v>20</v>
-      </c>
-      <c r="D24">
-        <v>6</v>
-      </c>
-      <c r="E24">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>OUTPUT9.xlsx</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>JANSSEN</t>
-        </is>
-      </c>
-      <c r="C25">
-        <v>91</v>
-      </c>
-      <c r="D25">
-        <v>36</v>
-      </c>
-      <c r="E25">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>OUTPUT9.xlsx</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>NOVAVAX</t>
-        </is>
-      </c>
-      <c r="C26">
-        <v>165</v>
-      </c>
-      <c r="D26">
-        <v>57</v>
-      </c>
-      <c r="E26">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>OUTPUT9.xlsx</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>MODERNA BIVALENT</t>
-        </is>
-      </c>
-      <c r="C27">
-        <v>68</v>
-      </c>
-      <c r="D27">
-        <v>33</v>
-      </c>
-      <c r="E27">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>OUTPUT9.xlsx</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>PFIZER-BIONTECH BIVALENT</t>
-        </is>
-      </c>
-      <c r="C28">
-        <v>84</v>
-      </c>
-      <c r="D28">
-        <v>32</v>
-      </c>
-      <c r="E28">
         <v>52</v>
       </c>
     </row>

</xml_diff>